<commit_message>
Auto stash before merge of "develop" and "origin/develop"
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C0D64-7DBC-460F-B7A8-761BCC4B2C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="ETLE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -82,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,19 +447,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -468,42 +467,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -514,23 +513,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6985D34C-6EF7-4849-ACAF-BBEB94FFD830}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -538,12 +537,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>-5</v>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Auto stash before merge of "develop" and "origin/develop""
This reverts commit 946599780226d051aa143b72ffc614abd1a2ad25.
</commit_message>
<xml_diff>
--- a/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
+++ b/InputData/elec/ETLE/Electricity Technology Logit Exponent.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\ETLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C0D64-7DBC-460F-B7A8-761BCC4B2C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="ETLE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,19 +448,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -467,42 +468,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -513,23 +514,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6985D34C-6EF7-4849-ACAF-BBEB94FFD830}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -537,12 +538,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>